<commit_message>
COmmit al master blogs mas reciente
</commit_message>
<xml_diff>
--- a/excelejemplo.xlsx
+++ b/excelejemplo.xlsx
@@ -20,7 +20,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Invent equipos, precios mantto'!$A$2:$H$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Invent equipos, precios mantto'!$A$2:$H$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
   <si>
     <t>SEDE</t>
   </si>
@@ -458,6 +458,24 @@
   <si>
     <t>no</t>
   </si>
+  <si>
+    <t>JJ</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
 </sst>
 </file>
 
@@ -466,13 +484,13 @@
   <numFmts count="7">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,16 +536,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1049,7 +1057,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1067,79 +1075,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,179 +1156,179 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="5" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="5" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="6" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="6" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="6" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="6" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="6" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="6" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="6" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="6" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="6" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="6" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1330,7 +1338,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1339,7 +1347,7 @@
     <xf numFmtId="44" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1348,7 +1356,7 @@
     <xf numFmtId="44" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1360,7 +1368,7 @@
     <xf numFmtId="44" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1369,7 +1377,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1378,7 +1386,7 @@
     <xf numFmtId="44" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1387,7 +1395,7 @@
     <xf numFmtId="44" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1399,49 +1407,49 @@
     <xf numFmtId="44" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="5" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="5" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="6" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1450,15 +1458,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1477,56 +1485,56 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1626,7 +1634,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1698,9 +1706,6 @@
           <cell r="N80">
             <v>0.53604803823901481</v>
           </cell>
-          <cell r="O80">
-            <v>0</v>
-          </cell>
           <cell r="P80">
             <v>39030605.210000001</v>
           </cell>
@@ -1850,9 +1855,6 @@
           <cell r="N81">
             <v>0.15326882988051116</v>
           </cell>
-          <cell r="O81">
-            <v>0</v>
-          </cell>
           <cell r="P81">
             <v>199505248</v>
           </cell>
@@ -2002,9 +2004,6 @@
           <cell r="N82">
             <v>0.54504135215335836</v>
           </cell>
-          <cell r="O82">
-            <v>0</v>
-          </cell>
           <cell r="P82">
             <v>34968000</v>
           </cell>
@@ -2153,9 +2152,6 @@
           </cell>
           <cell r="N83">
             <v>7.3251664840661077E-2</v>
-          </cell>
-          <cell r="O83">
-            <v>0</v>
           </cell>
           <cell r="P83">
             <v>14267424.404937617</v>
@@ -3195,7 +3191,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Dell" refreshedDate="44589.575015046299" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="2428">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:H7" sheet="Invent equipos, precios mantto"/>
+    <worksheetSource ref="A2:H9" sheet="Invent equipos, precios mantto"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="SEDE" numFmtId="0">
@@ -3253,7 +3249,7 @@
     <cacheField name="ACTIVO FIJO" numFmtId="0">
       <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1930" maxValue="2107452"/>
     </cacheField>
-    <cacheField name="VAALOR MANTTO 2022 " numFmtId="166">
+    <cacheField name="VAALOR MANTTO 2022 " numFmtId="164">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="9506" maxValue="152093"/>
     </cacheField>
   </cacheFields>
@@ -27711,7 +27707,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Suma de VAALOR MANTTO 2022 " fld="7" baseField="0" baseItem="0" numFmtId="167"/>
+    <dataField name="Suma de VAALOR MANTTO 2022 " fld="7" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="1">
     <format dxfId="9">
@@ -28027,12 +28023,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28190,7 +28186,7 @@
         <v>38023</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -28198,36 +28194,88 @@
         <v>139</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="7">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="7">
+        <v>234560000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H9" s="7">
         <v>38023</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="G9" s="11" t="s">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="G11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="12">
-        <f>SUM(H3:H8)</f>
-        <v>190115</v>
+      <c r="H11" s="12">
+        <f>SUM(H3:H10)</f>
+        <v>234850115</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28541,10 +28589,10 @@
   <dimension ref="A1:BA75"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28600,91 +28648,91 @@
     </row>
     <row r="2" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:53" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="163" t="s">
+      <c r="C3" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="164"/>
-      <c r="E3" s="165"/>
-      <c r="F3" s="164" t="s">
+      <c r="D3" s="159"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="159" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="163" t="s">
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="170" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="164"/>
-      <c r="K3" s="165"/>
-      <c r="L3" s="169" t="s">
+      <c r="J3" s="159"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="169"/>
-      <c r="N3" s="169"/>
-      <c r="O3" s="163" t="s">
+      <c r="M3" s="163"/>
+      <c r="N3" s="163"/>
+      <c r="O3" s="170" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="164"/>
-      <c r="Q3" s="165"/>
-      <c r="R3" s="164" t="s">
+      <c r="P3" s="159"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="159" t="s">
         <v>68</v>
       </c>
-      <c r="S3" s="164"/>
-      <c r="T3" s="164"/>
-      <c r="U3" s="166" t="s">
+      <c r="S3" s="159"/>
+      <c r="T3" s="159"/>
+      <c r="U3" s="160" t="s">
         <v>69</v>
       </c>
-      <c r="V3" s="167"/>
-      <c r="W3" s="168"/>
-      <c r="X3" s="169" t="s">
+      <c r="V3" s="161"/>
+      <c r="W3" s="162"/>
+      <c r="X3" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="Y3" s="169"/>
-      <c r="Z3" s="169"/>
-      <c r="AA3" s="163" t="s">
+      <c r="Y3" s="163"/>
+      <c r="Z3" s="163"/>
+      <c r="AA3" s="170" t="s">
         <v>71</v>
       </c>
-      <c r="AB3" s="164"/>
-      <c r="AC3" s="165"/>
-      <c r="AD3" s="164" t="s">
+      <c r="AB3" s="159"/>
+      <c r="AC3" s="171"/>
+      <c r="AD3" s="159" t="s">
         <v>72</v>
       </c>
-      <c r="AE3" s="164"/>
-      <c r="AF3" s="164"/>
-      <c r="AG3" s="163" t="s">
+      <c r="AE3" s="159"/>
+      <c r="AF3" s="159"/>
+      <c r="AG3" s="170" t="s">
         <v>73</v>
       </c>
-      <c r="AH3" s="164"/>
-      <c r="AI3" s="165"/>
-      <c r="AJ3" s="169" t="s">
+      <c r="AH3" s="159"/>
+      <c r="AI3" s="171"/>
+      <c r="AJ3" s="163" t="s">
         <v>74</v>
       </c>
-      <c r="AK3" s="169"/>
-      <c r="AL3" s="169"/>
-      <c r="AM3" s="163" t="s">
+      <c r="AK3" s="163"/>
+      <c r="AL3" s="163"/>
+      <c r="AM3" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="AN3" s="164"/>
-      <c r="AO3" s="165"/>
-      <c r="AP3" s="164" t="s">
+      <c r="AN3" s="159"/>
+      <c r="AO3" s="171"/>
+      <c r="AP3" s="159" t="s">
         <v>76</v>
       </c>
-      <c r="AQ3" s="164"/>
-      <c r="AR3" s="164"/>
-      <c r="AS3" s="166" t="s">
+      <c r="AQ3" s="159"/>
+      <c r="AR3" s="159"/>
+      <c r="AS3" s="160" t="s">
         <v>77</v>
       </c>
-      <c r="AT3" s="167"/>
-      <c r="AU3" s="168"/>
-      <c r="AV3" s="169" t="s">
+      <c r="AT3" s="161"/>
+      <c r="AU3" s="162"/>
+      <c r="AV3" s="163" t="s">
         <v>78</v>
       </c>
-      <c r="AW3" s="169"/>
-      <c r="AX3" s="169"/>
-      <c r="AY3" s="170" t="s">
+      <c r="AW3" s="163"/>
+      <c r="AX3" s="163"/>
+      <c r="AY3" s="164" t="s">
         <v>79</v>
       </c>
-      <c r="AZ3" s="171"/>
-      <c r="BA3" s="172"/>
+      <c r="AZ3" s="165"/>
+      <c r="BA3" s="166"/>
     </row>
     <row r="4" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
@@ -28842,7 +28890,7 @@
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A5" s="159" t="s">
+      <c r="A5" s="167" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -28896,8 +28944,7 @@
         <v>0.53604803823901481</v>
       </c>
       <c r="O5" s="26">
-        <f>'[1]Budget ZONA NORTE'!O80</f>
-        <v>0</v>
+        <v>3232</v>
       </c>
       <c r="P5" s="27">
         <f>'[1]Budget ZONA NORTE'!P80</f>
@@ -29053,7 +29100,7 @@
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A6" s="160"/>
+      <c r="A6" s="168"/>
       <c r="B6" s="37" t="s">
         <v>100</v>
       </c>
@@ -29105,8 +29152,7 @@
         <v>0.15326882988051116</v>
       </c>
       <c r="O6" s="38">
-        <f>'[1]Budget ZONA NORTE'!O81</f>
-        <v>0</v>
+        <v>3232</v>
       </c>
       <c r="P6" s="39">
         <f>'[1]Budget ZONA NORTE'!P81</f>
@@ -29262,7 +29308,7 @@
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A7" s="160"/>
+      <c r="A7" s="168"/>
       <c r="B7" s="37" t="s">
         <v>101</v>
       </c>
@@ -29314,8 +29360,7 @@
         <v>0.54504135215335836</v>
       </c>
       <c r="O7" s="38">
-        <f>'[1]Budget ZONA NORTE'!O82</f>
-        <v>0</v>
+        <v>3232</v>
       </c>
       <c r="P7" s="39">
         <f>'[1]Budget ZONA NORTE'!P82</f>
@@ -29471,7 +29516,7 @@
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A8" s="160"/>
+      <c r="A8" s="168"/>
       <c r="B8" s="37" t="s">
         <v>102</v>
       </c>
@@ -29523,8 +29568,7 @@
         <v>7.3251664840661077E-2</v>
       </c>
       <c r="O8" s="38">
-        <f>'[1]Budget ZONA NORTE'!O83</f>
-        <v>0</v>
+        <v>444</v>
       </c>
       <c r="P8" s="39">
         <f>'[1]Budget ZONA NORTE'!P83</f>
@@ -29680,7 +29724,7 @@
       </c>
     </row>
     <row r="9" spans="1:53" s="62" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="173"/>
+      <c r="A9" s="169"/>
       <c r="B9" s="49" t="s">
         <v>103</v>
       </c>
@@ -29889,7 +29933,7 @@
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A10" s="159" t="s">
+      <c r="A10" s="167" t="s">
         <v>104</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -30100,7 +30144,7 @@
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A11" s="160"/>
+      <c r="A11" s="168"/>
       <c r="B11" s="37" t="s">
         <v>100</v>
       </c>
@@ -30309,7 +30353,7 @@
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A12" s="160"/>
+      <c r="A12" s="168"/>
       <c r="B12" s="37" t="s">
         <v>101</v>
       </c>
@@ -30518,7 +30562,7 @@
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A13" s="160"/>
+      <c r="A13" s="168"/>
       <c r="B13" s="37" t="s">
         <v>102</v>
       </c>
@@ -30727,7 +30771,7 @@
       </c>
     </row>
     <row r="14" spans="1:53" s="62" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="161"/>
+      <c r="A14" s="172"/>
       <c r="B14" s="85" t="s">
         <v>105</v>
       </c>
@@ -30937,7 +30981,7 @@
     </row>
     <row r="15" spans="1:53" s="97" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="167" t="s">
         <v>106</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -30993,7 +31037,7 @@
       </c>
       <c r="O16" s="98">
         <f>O5+O10</f>
-        <v>0</v>
+        <v>3232</v>
       </c>
       <c r="P16" s="99">
         <f>P5+P10</f>
@@ -31001,7 +31045,7 @@
       </c>
       <c r="Q16" s="100">
         <f>+O16/P16</f>
-        <v>0</v>
+        <v>5.6931724383451403E-5</v>
       </c>
       <c r="R16" s="107">
         <f>R5+R10</f>
@@ -31149,7 +31193,7 @@
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A17" s="160"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="37" t="s">
         <v>100</v>
       </c>
@@ -31203,7 +31247,7 @@
       </c>
       <c r="O17" s="111">
         <f t="shared" ref="O17:P20" si="10">O6+O11</f>
-        <v>0</v>
+        <v>3232</v>
       </c>
       <c r="P17" s="112">
         <f t="shared" si="10"/>
@@ -31211,7 +31255,7 @@
       </c>
       <c r="Q17" s="113">
         <f t="shared" ref="Q17:Q20" si="11">+O17/P17</f>
-        <v>0</v>
+        <v>8.1060265056633241E-6</v>
       </c>
       <c r="R17" s="120">
         <f t="shared" ref="R17:S20" si="12">R6+R11</f>
@@ -31359,7 +31403,7 @@
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A18" s="160"/>
+      <c r="A18" s="168"/>
       <c r="B18" s="37" t="s">
         <v>101</v>
       </c>
@@ -31413,7 +31457,7 @@
       </c>
       <c r="O18" s="111">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3232</v>
       </c>
       <c r="P18" s="112">
         <f t="shared" si="10"/>
@@ -31421,7 +31465,7 @@
       </c>
       <c r="Q18" s="113">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5.1666120485009308E-5</v>
       </c>
       <c r="R18" s="120">
         <f t="shared" si="12"/>
@@ -31569,7 +31613,7 @@
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A19" s="160"/>
+      <c r="A19" s="168"/>
       <c r="B19" s="37" t="s">
         <v>102</v>
       </c>
@@ -31623,7 +31667,7 @@
       </c>
       <c r="O19" s="111">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>444</v>
       </c>
       <c r="P19" s="112">
         <f t="shared" si="10"/>
@@ -31631,7 +31675,7 @@
       </c>
       <c r="Q19" s="113">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8.0844379181862928E-6</v>
       </c>
       <c r="R19" s="120">
         <f t="shared" si="12"/>
@@ -31779,7 +31823,7 @@
       </c>
     </row>
     <row r="20" spans="1:53" s="62" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="161"/>
+      <c r="A20" s="172"/>
       <c r="B20" s="85" t="s">
         <v>107</v>
       </c>
@@ -32089,10 +32133,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="162" t="s">
+      <c r="B38" s="173" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="162"/>
+      <c r="C38" s="173"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" s="139" t="s">
@@ -32124,10 +32168,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
-      <c r="B44" s="162" t="s">
+      <c r="B44" s="173" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="162"/>
+      <c r="C44" s="173"/>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -32559,6 +32603,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="R3:T3"/>
     <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="AS3:AU3"/>
     <mergeCell ref="AV3:AX3"/>
@@ -32575,12 +32625,6 @@
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <conditionalFormatting sqref="E9">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="between">

</xml_diff>

<commit_message>
agregado continido mejor al master
</commit_message>
<xml_diff>
--- a/excelejemplo.xlsx
+++ b/excelejemplo.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="148">
   <si>
     <t>SEDE</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>AA</t>
+  </si>
+  <si>
+    <t>PROVISION ABRIL</t>
+  </si>
+  <si>
+    <t>PROVISION MAYO</t>
   </si>
 </sst>
 </file>
@@ -1054,12 +1060,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1491,7 +1498,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1515,29 +1540,16 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Moneda" xfId="3" builtinId="4"/>
     <cellStyle name="Moneda 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
@@ -28023,12 +28035,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28276,6 +28288,22 @@
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="175" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="174">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="175" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="174">
+        <v>70000000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28592,7 +28620,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28648,91 +28676,91 @@
     </row>
     <row r="2" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:53" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="170" t="s">
+      <c r="C3" s="163" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="159"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="159" t="s">
+      <c r="D3" s="164"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="159"/>
-      <c r="H3" s="159"/>
-      <c r="I3" s="170" t="s">
+      <c r="G3" s="164"/>
+      <c r="H3" s="164"/>
+      <c r="I3" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="159"/>
-      <c r="K3" s="171"/>
-      <c r="L3" s="163" t="s">
+      <c r="J3" s="164"/>
+      <c r="K3" s="165"/>
+      <c r="L3" s="169" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="163"/>
-      <c r="N3" s="163"/>
-      <c r="O3" s="170" t="s">
+      <c r="M3" s="169"/>
+      <c r="N3" s="169"/>
+      <c r="O3" s="163" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="159"/>
-      <c r="Q3" s="171"/>
-      <c r="R3" s="159" t="s">
+      <c r="P3" s="164"/>
+      <c r="Q3" s="165"/>
+      <c r="R3" s="164" t="s">
         <v>68</v>
       </c>
-      <c r="S3" s="159"/>
-      <c r="T3" s="159"/>
-      <c r="U3" s="160" t="s">
+      <c r="S3" s="164"/>
+      <c r="T3" s="164"/>
+      <c r="U3" s="166" t="s">
         <v>69</v>
       </c>
-      <c r="V3" s="161"/>
-      <c r="W3" s="162"/>
-      <c r="X3" s="163" t="s">
+      <c r="V3" s="167"/>
+      <c r="W3" s="168"/>
+      <c r="X3" s="169" t="s">
         <v>70</v>
       </c>
-      <c r="Y3" s="163"/>
-      <c r="Z3" s="163"/>
-      <c r="AA3" s="170" t="s">
+      <c r="Y3" s="169"/>
+      <c r="Z3" s="169"/>
+      <c r="AA3" s="163" t="s">
         <v>71</v>
       </c>
-      <c r="AB3" s="159"/>
-      <c r="AC3" s="171"/>
-      <c r="AD3" s="159" t="s">
+      <c r="AB3" s="164"/>
+      <c r="AC3" s="165"/>
+      <c r="AD3" s="164" t="s">
         <v>72</v>
       </c>
-      <c r="AE3" s="159"/>
-      <c r="AF3" s="159"/>
-      <c r="AG3" s="170" t="s">
+      <c r="AE3" s="164"/>
+      <c r="AF3" s="164"/>
+      <c r="AG3" s="163" t="s">
         <v>73</v>
       </c>
-      <c r="AH3" s="159"/>
-      <c r="AI3" s="171"/>
-      <c r="AJ3" s="163" t="s">
+      <c r="AH3" s="164"/>
+      <c r="AI3" s="165"/>
+      <c r="AJ3" s="169" t="s">
         <v>74</v>
       </c>
-      <c r="AK3" s="163"/>
-      <c r="AL3" s="163"/>
-      <c r="AM3" s="170" t="s">
+      <c r="AK3" s="169"/>
+      <c r="AL3" s="169"/>
+      <c r="AM3" s="163" t="s">
         <v>75</v>
       </c>
-      <c r="AN3" s="159"/>
-      <c r="AO3" s="171"/>
-      <c r="AP3" s="159" t="s">
+      <c r="AN3" s="164"/>
+      <c r="AO3" s="165"/>
+      <c r="AP3" s="164" t="s">
         <v>76</v>
       </c>
-      <c r="AQ3" s="159"/>
-      <c r="AR3" s="159"/>
-      <c r="AS3" s="160" t="s">
+      <c r="AQ3" s="164"/>
+      <c r="AR3" s="164"/>
+      <c r="AS3" s="166" t="s">
         <v>77</v>
       </c>
-      <c r="AT3" s="161"/>
-      <c r="AU3" s="162"/>
-      <c r="AV3" s="163" t="s">
+      <c r="AT3" s="167"/>
+      <c r="AU3" s="168"/>
+      <c r="AV3" s="169" t="s">
         <v>78</v>
       </c>
-      <c r="AW3" s="163"/>
-      <c r="AX3" s="163"/>
-      <c r="AY3" s="164" t="s">
+      <c r="AW3" s="169"/>
+      <c r="AX3" s="169"/>
+      <c r="AY3" s="170" t="s">
         <v>79</v>
       </c>
-      <c r="AZ3" s="165"/>
-      <c r="BA3" s="166"/>
+      <c r="AZ3" s="171"/>
+      <c r="BA3" s="172"/>
     </row>
     <row r="4" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
@@ -28890,7 +28918,7 @@
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A5" s="167" t="s">
+      <c r="A5" s="159" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -29100,7 +29128,7 @@
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A6" s="168"/>
+      <c r="A6" s="160"/>
       <c r="B6" s="37" t="s">
         <v>100</v>
       </c>
@@ -29308,7 +29336,7 @@
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A7" s="168"/>
+      <c r="A7" s="160"/>
       <c r="B7" s="37" t="s">
         <v>101</v>
       </c>
@@ -29516,7 +29544,7 @@
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A8" s="168"/>
+      <c r="A8" s="160"/>
       <c r="B8" s="37" t="s">
         <v>102</v>
       </c>
@@ -29724,7 +29752,7 @@
       </c>
     </row>
     <row r="9" spans="1:53" s="62" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="169"/>
+      <c r="A9" s="173"/>
       <c r="B9" s="49" t="s">
         <v>103</v>
       </c>
@@ -29933,7 +29961,7 @@
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A10" s="167" t="s">
+      <c r="A10" s="159" t="s">
         <v>104</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -30144,7 +30172,7 @@
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A11" s="168"/>
+      <c r="A11" s="160"/>
       <c r="B11" s="37" t="s">
         <v>100</v>
       </c>
@@ -30353,7 +30381,7 @@
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A12" s="168"/>
+      <c r="A12" s="160"/>
       <c r="B12" s="37" t="s">
         <v>101</v>
       </c>
@@ -30562,7 +30590,7 @@
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A13" s="168"/>
+      <c r="A13" s="160"/>
       <c r="B13" s="37" t="s">
         <v>102</v>
       </c>
@@ -30771,7 +30799,7 @@
       </c>
     </row>
     <row r="14" spans="1:53" s="62" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="172"/>
+      <c r="A14" s="161"/>
       <c r="B14" s="85" t="s">
         <v>105</v>
       </c>
@@ -30981,7 +31009,7 @@
     </row>
     <row r="15" spans="1:53" s="97" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A16" s="167" t="s">
+      <c r="A16" s="159" t="s">
         <v>106</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -31193,7 +31221,7 @@
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A17" s="168"/>
+      <c r="A17" s="160"/>
       <c r="B17" s="37" t="s">
         <v>100</v>
       </c>
@@ -31403,7 +31431,7 @@
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A18" s="168"/>
+      <c r="A18" s="160"/>
       <c r="B18" s="37" t="s">
         <v>101</v>
       </c>
@@ -31613,7 +31641,7 @@
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A19" s="168"/>
+      <c r="A19" s="160"/>
       <c r="B19" s="37" t="s">
         <v>102</v>
       </c>
@@ -31823,7 +31851,7 @@
       </c>
     </row>
     <row r="20" spans="1:53" s="62" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="172"/>
+      <c r="A20" s="161"/>
       <c r="B20" s="85" t="s">
         <v>107</v>
       </c>
@@ -32044,6 +32072,14 @@
         <v>1.1298293783354714</v>
       </c>
       <c r="AZ21" s="135"/>
+    </row>
+    <row r="22" spans="1:53" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L22" s="176" t="s">
+        <v>147</v>
+      </c>
+      <c r="M22" s="177">
+        <v>600000</v>
+      </c>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">
@@ -32133,10 +32169,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="173" t="s">
+      <c r="B38" s="162" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="173"/>
+      <c r="C38" s="162"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" s="139" t="s">
@@ -32168,10 +32204,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
-      <c r="B44" s="173" t="s">
+      <c r="B44" s="162" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="173"/>
+      <c r="C44" s="162"/>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -32603,12 +32639,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="R3:T3"/>
     <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="AS3:AU3"/>
     <mergeCell ref="AV3:AX3"/>
@@ -32625,6 +32655,12 @@
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <conditionalFormatting sqref="E9">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="between">

</xml_diff>